<commit_message>
Add file from private repo
</commit_message>
<xml_diff>
--- a/CryCompanywiseStockReport_1.xlsx
+++ b/CryCompanywiseStockReport_1.xlsx
@@ -832,24 +832,24 @@
         <v>9</v>
       </c>
       <c r="B15" t="n">
-        <v>59408</v>
+        <v>47438</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>SIG-3W Lilliput LED Torch &amp;amp; Table Lamp</t>
+          <t>SIG-3w Lilliput LED Torch &amp;amp; Table Lamp</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>388.17</v>
+        <v>401.81</v>
       </c>
       <c r="E15" t="n">
-        <v>463.78</v>
+        <v>480.05</v>
       </c>
       <c r="F15" t="n">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="G15" t="n">
-        <v>10868.76</v>
+        <v>803.62</v>
       </c>
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr"/>
@@ -863,24 +863,24 @@
         <v>10</v>
       </c>
       <c r="B16" t="n">
-        <v>47438</v>
+        <v>59408</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>SIG-3w Lilliput LED Torch &amp;amp; Table Lamp</t>
+          <t>SIG-3W Lilliput LED Torch &amp;amp; Table Lamp</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>401.81</v>
+        <v>388.17</v>
       </c>
       <c r="E16" t="n">
-        <v>480.05</v>
+        <v>463.78</v>
       </c>
       <c r="F16" t="n">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="G16" t="n">
-        <v>803.62</v>
+        <v>10868.76</v>
       </c>
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr"/>

</xml_diff>